<commit_message>
Intellicage and VitalView data analysis
- Updated the Intellicage plots to the paper
- Updated the ER400 (VitalView) plots to the paper
- Fix a bug in plotter
</commit_message>
<xml_diff>
--- a/src/analysis_examples/er4000/results_er4000/animal_01/cosinor_animal_01_act.xlsx
+++ b/src/analysis_examples/er4000/results_er4000/animal_01/cosinor_animal_01_act.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,39 +571,39 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>24.06000000000032</v>
+        <v>24.10000000000033</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>4.169331546677313e-12</v>
+        <v>1.110223024625157e-16</v>
       </c>
       <c r="H2" t="n">
-        <v>1.820717489818968e-11</v>
+        <v>4.662353909187009e-16</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
-        <v>182.0843377523794</v>
+        <v>452.9059165541908</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[131.6818846021116, 232.48679090264716]</t>
+          <t>[361.6305809805874, 544.1812521277941]</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>2.941091814534502e-11</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>3.676364768168128e-11</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>1.553500271144503</v>
+        <v>1.566079220708425</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>[1.2390265320464255, 1.8679740102425804]</t>
+          <t>[1.3522370781217319, 1.7799213632951183]</t>
         </is>
       </c>
       <c r="Q2" t="n">
@@ -613,11 +613,11 @@
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>592.8083241542569</v>
+        <v>823.1329243291839</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>[560.450217330221, 625.1664309782927]</t>
+          <t>[762.0787323913034, 884.1871162670643]</t>
         </is>
       </c>
       <c r="U2" t="n">
@@ -627,13 +627,13 @@
         <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>18.11123123123147</v>
+        <v>18.09309309309334</v>
       </c>
       <c r="X2" t="n">
-        <v>16.90702702702725</v>
+        <v>17.27287287287311</v>
       </c>
       <c r="Y2" t="n">
-        <v>19.31543543543569</v>
+        <v>18.91331331331357</v>
       </c>
     </row>
     <row r="3">
@@ -645,14 +645,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2_control_dd</t>
+          <t>2_induction_dd</t>
         </is>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>23.9400000000003</v>
+        <v>23.85000000000029</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -661,16 +661,18 @@
         <v>1.110223024625157e-16</v>
       </c>
       <c r="H3" t="n">
-        <v>6.417474130781252e-16</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
+        <v>4.662353909187009e-16</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.001266727310926918</v>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
-        <v>187.4161142458028</v>
+        <v>253.8204589722343</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[161.90196086728054, 212.93026762432498]</t>
+          <t>[213.64159811621641, 293.99931982825217]</t>
         </is>
       </c>
       <c r="M3" t="n">
@@ -680,11 +682,11 @@
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>1.704447665911579</v>
+        <v>2.270500396288118</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>[1.553500271144503, 1.8553950606786556]</t>
+          <t>[2.11955300152104, 2.421447791055196]</t>
         </is>
       </c>
       <c r="Q3" t="n">
@@ -694,11 +696,11 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>671.1481946435262</v>
+        <v>707.0312904389067</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>[655.0497603902143, 687.246628896838]</t>
+          <t>[686.6019064862714, 727.4606743915419]</t>
         </is>
       </c>
       <c r="U3" t="n">
@@ -708,13 +710,13 @@
         <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>17.44576576576599</v>
+        <v>15.23153153153172</v>
       </c>
       <c r="X3" t="n">
-        <v>16.87063063063085</v>
+        <v>14.65855855855873</v>
       </c>
       <c r="Y3" t="n">
-        <v>18.02090090090113</v>
+        <v>15.8045045045047</v>
       </c>
     </row>
     <row r="4">
@@ -726,60 +728,62 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3_induction_dd</t>
+          <t>3_hypo_dd</t>
         </is>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>23.96000000000031</v>
+        <v>23.70000000000027</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
       <c r="G4" t="n">
+        <v>1.159506934911292e-10</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2.806673367410086e-10</v>
+      </c>
+      <c r="I4" t="n">
         <v>1.110223024625157e-16</v>
       </c>
-      <c r="H4" t="n">
-        <v>6.417474130781252e-16</v>
-      </c>
-      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
-        <v>159.3460031219248</v>
+        <v>129.6573846840802</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[125.15085677004834, 193.54114947380117]</t>
+          <t>[85.94007736177969, 173.37469200638066]</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>1.035688845796301e-08</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>1.035688845796301e-08</v>
       </c>
       <c r="O4" t="n">
-        <v>2.748500479717197</v>
+        <v>1.314500229429964</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>[2.5220793875665803, 2.974921571867813]</t>
+          <t>[0.9119738433844251, 1.7170266154755023]</t>
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>3.360474121194557e-10</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>3.360474121194557e-10</v>
       </c>
       <c r="S4" t="n">
-        <v>696.3287676463838</v>
+        <v>659.9581717835814</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>[677.6122500029471, 715.0452852898204]</t>
+          <t>[634.0343368885558, 685.882006678607]</t>
         </is>
       </c>
       <c r="U4" t="n">
@@ -789,13 +793,13 @@
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>13.47899899899917</v>
+        <v>18.74174174174195</v>
       </c>
       <c r="X4" t="n">
-        <v>12.61557557557573</v>
+        <v>17.22342342342362</v>
       </c>
       <c r="Y4" t="n">
-        <v>14.34242242242261</v>
+        <v>20.26006006006028</v>
       </c>
     </row>
     <row r="5">
@@ -803,64 +807,64 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4_hypo_dd</t>
+          <t>4_hypo_dl</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>23.41000000000022</v>
+        <v>25.52000000000055</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>5.112586465294555e-09</v>
+        <v>1.110223024625157e-16</v>
       </c>
       <c r="H5" t="n">
-        <v>1.424118792561158e-08</v>
+        <v>4.662353909187009e-16</v>
       </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="n">
-        <v>91.34228215815489</v>
+        <v>308.7776886554807</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[57.665791475801484, 125.01877284050829]</t>
+          <t>[256.9849643659252, 360.5704129450362]</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>1.520980537073058e-07</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>1.520980537073058e-07</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>0.1446579199851152</v>
+        <v>-2.138421425866927</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>[-0.2956053147521942, 0.5849211547224247]</t>
+          <t>[-2.3145267197618495, -1.962316131972004]</t>
         </is>
       </c>
       <c r="Q5" t="n">
-        <v>0.5188318200387818</v>
+        <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>0.5188318200387818</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>653.8175988542328</v>
+        <v>652.5730014004326</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>[633.6892113462069, 673.9459863622586]</t>
+          <t>[625.6545208149248, 679.4914819859405]</t>
         </is>
       </c>
       <c r="U5" t="n">
@@ -870,94 +874,13 @@
         <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>22.87103103103125</v>
+        <v>8.685485485485675</v>
       </c>
       <c r="X5" t="n">
-        <v>21.23069069069089</v>
+        <v>7.970210210210386</v>
       </c>
       <c r="Y5" t="n">
-        <v>24.51137137137161</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>5_hypo_dl</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>24.81000000000044</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.110223024625157e-16</v>
-      </c>
-      <c r="H6" t="n">
-        <v>6.417474130781252e-16</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
-        <v>192.8185410312198</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>[146.98527310844798, 238.65180895399152]</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>3.33066907387547e-15</v>
-      </c>
-      <c r="N6" t="n">
-        <v>5.551115123125783e-15</v>
-      </c>
-      <c r="O6" t="n">
-        <v>1.062921238151502</v>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>[0.823921196436963, 1.3019212798660416]</t>
-        </is>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" t="n">
-        <v>680.2908197224997</v>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>[656.0966880800273, 704.4849513649721]</t>
-        </is>
-      </c>
-      <c r="U6" t="n">
-        <v>0</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W6" t="n">
-        <v>20.61291291291327</v>
-      </c>
-      <c r="X6" t="n">
-        <v>19.66918918918953</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>21.55663663663702</v>
+        <v>9.400760760760964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>